<commit_message>
Aynı gün ve saatte sınav yapılıyor.Ama buna ekstra genişleme kuralları eklenicek.
</commit_message>
<xml_diff>
--- a/sinav_programi.xlsx
+++ b/sinav_programi.xlsx
@@ -9,8 +9,9 @@
   <sheets>
     <sheet name="Sınav Programı" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Oda Bazlı Görünüm" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Program Bilgileri" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Uyarılar" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Gün İstatistikleri" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Program Bilgileri" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Uyarılar" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,17 +477,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FEF203</t>
+          <t>AIT109</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Diferansiyel Denklemler</t>
+          <t>Atatürk İlkeleri ve İnkılap Tarihi I</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -494,7 +495,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>301, Büyük Amfi</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -507,25 +508,25 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MUH201</t>
+          <t>TDB107</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Nesneye Yönelik Programlama</t>
+          <t>Türk Dili I</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>303, EDA</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -538,17 +539,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AIT109</t>
+          <t>YDB117</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Atatürk İlkeleri ve İnkılap Tarihi I</t>
+          <t>İngilizce I</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -556,7 +557,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>305, 400</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -569,25 +570,25 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FEF113</t>
+          <t>FEF111</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Lineer Cebir</t>
+          <t>Fizik I</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>amfimsi, küçük amfi</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -600,17 +601,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MUH402</t>
+          <t>FEF113</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Bitirme Çalışması</t>
+          <t>Lineer Cebir</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-10-06</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -618,7 +619,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>100, 212</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -631,17 +632,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MUH301</t>
+          <t>FEF115</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Sayısal Yöntemler</t>
+          <t>Matematik I</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -649,7 +650,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>Yazılım Amfi, Jeofizik Amfi</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -662,25 +663,25 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BLM305</t>
+          <t>BLM101</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>İşletim Sistemleri</t>
+          <t>Bilgisayar Laboratuvarı I</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t xml:space="preserve">amfilerden biri, HKAmsı </t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -693,17 +694,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BLM441</t>
+          <t>BLM103</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mobil Programlama</t>
+          <t>Bilgisayar Mühendisliğine Giriş</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-10-09</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -711,7 +712,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>afi, dersllik</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -724,17 +725,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BLM417</t>
+          <t>BLM105</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Programlanabilir Yapılar</t>
+          <t xml:space="preserve">Programlama I </t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -742,7 +743,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>enes, adsas</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -755,25 +756,25 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BLM421</t>
+          <t>FEF203</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Yazılım Proje Yönetimi</t>
+          <t>Diferansiyel Denklemler</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>oooo, mmmm</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -786,17 +787,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BLM401</t>
+          <t>MUH201</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Bilgisayar Ağları</t>
+          <t>Nesneye Yönelik Programlama</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-10-12</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -804,7 +805,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>ss, sdsdsd</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -817,17 +818,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BLM307</t>
+          <t>BLM207</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yazılım Laboratuvarı I </t>
+          <t>Veri Yapıları ve Algoritmaları</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -835,7 +836,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>aa, fgfg</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -848,25 +849,25 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BLM309</t>
+          <t>BLM209</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Staj II</t>
+          <t xml:space="preserve">Programlama Laboratuvarı - I </t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>a, sd, a</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -879,17 +880,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>BLM323</t>
+          <t>BLM211</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Bilgi Güvenliği ve Kriptografi</t>
+          <t>Mantıksal Tasarım ve Uygulamalar</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -897,7 +898,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>301, Büyük Amfi</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -910,25 +911,25 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>BLM411</t>
+          <t>BLM205</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Bilgisayar Semineri</t>
+          <t>Ayrık Matematik</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>303, EDA</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -941,25 +942,25 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>BLM207</t>
+          <t>BLM213</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Veri Yapıları ve Algoritmaları</t>
+          <t>Staj I</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>305, 400</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -972,25 +973,25 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>BLM205</t>
+          <t>MUH301</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Ayrık Matematik</t>
+          <t>Sayısal Yöntemler</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>amfimsi, küçük amfi</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -1003,25 +1004,25 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>FEF115</t>
+          <t>BLM303</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Matematik I</t>
+          <t>İşaret ve Sistemler</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>100, 212</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -1034,25 +1035,25 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BLM103</t>
+          <t>BLM305</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Bilgisayar Mühendisliğine Giriş</t>
+          <t>İşletim Sistemleri</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>Yazılım Amfi, Jeofizik Amfi</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -1065,17 +1066,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>BLM429</t>
+          <t>BLM325</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Veri Madenciliğine Giriş</t>
+          <t>Mikroişlemci Sistemleri</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1083,7 +1084,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t xml:space="preserve">amfilerden biri, HKAmsı </t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1096,25 +1097,25 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>BLM451</t>
+          <t>BLM307</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Derin Öğrenmenin Temelleri</t>
+          <t xml:space="preserve">Yazılım Laboratuvarı I </t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>afi, dersllik</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1127,31 +1128,558 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>BLM309</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Staj II</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>enes, adsas</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>100</v>
+      </c>
+      <c r="G23" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>BLM323</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Bilgi Güvenliği ve Kriptografi</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>oooo, mmmm</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>100</v>
+      </c>
+      <c r="G24" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>BLM321</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Robotlar için Matematik Temelleri</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>ss, sdsdsd</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>100</v>
+      </c>
+      <c r="G25" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>MUH403</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Araştırma Problemleri</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>aa, fgfg</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>100</v>
+      </c>
+      <c r="G26" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>MUH402</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Bitirme Çalışması</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>a, sd, a</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>100</v>
+      </c>
+      <c r="G27" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>BLM401</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Bilgisayar Ağları</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>2</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>301, Büyük Amfi</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>100</v>
+      </c>
+      <c r="G28" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>BLM405</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>İş Hayatı ve İş Güvenliğine Hazırlık</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>303, EDA</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>100</v>
+      </c>
+      <c r="G29" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>BLM417</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Programlanabilir Yapılar</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>305, 400</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>100</v>
+      </c>
+      <c r="G30" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>BLM421</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Yazılım Proje Yönetimi</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>amfimsi, küçük amfi</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>100</v>
+      </c>
+      <c r="G31" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>BLM449</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Bilgisayarlı Görmenin Temelleri</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>2</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>100, 212</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>100</v>
+      </c>
+      <c r="G32" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>BLM429</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Veri Madenciliğine Giriş</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Yazılım Amfi, Jeofizik Amfi</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>100</v>
+      </c>
+      <c r="G33" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>BLM441</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Mobil Programlama</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>2</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">amfilerden biri, HKAmsı </t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>100</v>
+      </c>
+      <c r="G34" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>MUH445</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Mühendisler için İstatistik</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>2</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>afi, dersllik</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>100</v>
+      </c>
+      <c r="G35" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>BLM451</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Derin Öğrenmenin Temelleri</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>2</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>enes, adsas</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>100</v>
+      </c>
+      <c r="G36" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>BLM443</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Doğal Dil İşleme ve Metin Madenciliğine Giriş</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>2</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>oooo, mmmm</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>100</v>
+      </c>
+      <c r="G37" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>MUH413</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Gezgin Robotlara Giriş</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>2</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>ss, sdsdsd</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>100</v>
+      </c>
+      <c r="G38" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
           <t>BLM435</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B39" t="inlineStr">
         <is>
           <t>Biyoinformatiğe Giriş</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>2025-10-21</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
         <v>2</v>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>amfilerden biri</t>
-        </is>
-      </c>
-      <c r="F23" t="n">
-        <v>100</v>
-      </c>
-      <c r="G23" t="n">
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>aa, fgfg</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>100</v>
+      </c>
+      <c r="G39" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>BLM411</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Bilgisayar Semineri</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>2</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>a, sd, a</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>100</v>
+      </c>
+      <c r="G40" t="n">
         <v>75</v>
       </c>
     </row>
@@ -1166,7 +1694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1197,7 +1725,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Öğrenci Sayısı</t>
+          <t>Öğrenci</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -1209,17 +1737,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>301, Büyük Amfi</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Sabah (09:00-10:15)</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1239,22 +1767,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>303, EDA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Akşam (14:00-15:15)</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Lineer Cebir</t>
+          <t>Türk Dili I</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -1269,22 +1797,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>305, 400</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Sabah (09:00-10:15)</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Matematik I</t>
+          <t>İngilizce I</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -1299,22 +1827,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>amfimsi, küçük amfi</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Akşam (14:00-15:15)</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Bilgisayar Mühendisliğine Giriş</t>
+          <t>Fizik I</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -1329,22 +1857,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>100, 212</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Sabah (09:00-10:15)</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Diferansiyel Denklemler</t>
+          <t>Lineer Cebir</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -1359,22 +1887,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>Yazılım Amfi, Jeofizik Amfi</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Akşam (14:00-15:15)</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Nesneye Yönelik Programlama</t>
+          <t>Matematik I</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -1389,22 +1917,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t xml:space="preserve">amfilerden biri, HKAmsı </t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Sabah (09:00-10:15)</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Veri Yapıları ve Algoritmaları</t>
+          <t>Bilgisayar Laboratuvarı I</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -1419,22 +1947,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>afi, dersllik</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Akşam (14:00-15:15)</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Ayrık Matematik</t>
+          <t>Bilgisayar Mühendisliğine Giriş</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -1449,22 +1977,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>enes, adsas</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Sabah (09:00-10:15)</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Sayısal Yöntemler</t>
+          <t xml:space="preserve">Programlama I </t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -1479,22 +2007,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>oooo, mmmm</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Akşam (14:00-15:15)</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>İşletim Sistemleri</t>
+          <t>Diferansiyel Denklemler</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -1509,22 +2037,22 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>ss, sdsdsd</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Sabah (09:00-10:15)</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yazılım Laboratuvarı I </t>
+          <t>Nesneye Yönelik Programlama</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -1539,22 +2067,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>aa, fgfg</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Akşam (14:00-15:15)</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Staj II</t>
+          <t>Veri Yapıları ve Algoritmaları</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -1569,22 +2097,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>a, sd, a</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Öğle (11:00-12:15)</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Bilgi Güvenliği ve Kriptografi</t>
+          <t xml:space="preserve">Programlama Laboratuvarı - I </t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -1599,22 +2127,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>301, Büyük Amfi</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2025-10-06</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Sabah (09:00-10:15)</t>
+          <t>12:00-14:00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Bitirme Çalışması</t>
+          <t>Mantıksal Tasarım ve Uygulamalar</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -1629,22 +2157,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>303, EDA</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2025-10-12</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Sabah (09:00-10:15)</t>
+          <t>12:00-14:00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Bilgisayar Ağları</t>
+          <t>Ayrık Matematik</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -1659,22 +2187,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>305, 400</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Sabah (09:00-10:15)</t>
+          <t>12:00-14:00</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Programlanabilir Yapılar</t>
+          <t>Staj I</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -1689,22 +2217,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>amfimsi, küçük amfi</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Akşam (14:00-15:15)</t>
+          <t>12:00-14:00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Yazılım Proje Yönetimi</t>
+          <t>Sayısal Yöntemler</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -1719,22 +2247,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>100, 212</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Öğle (11:00-12:15)</t>
+          <t>12:00-14:00</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Veri Madenciliğine Giriş</t>
+          <t>İşaret ve Sistemler</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -1749,22 +2277,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>Yazılım Amfi, Jeofizik Amfi</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2025-10-09</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Sabah (09:00-10:15)</t>
+          <t>12:00-14:00</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Mobil Programlama</t>
+          <t>İşletim Sistemleri</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -1779,22 +2307,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t xml:space="preserve">amfilerden biri, HKAmsı </t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Sabah (09:00-10:15)</t>
+          <t>12:00-14:00</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Derin Öğrenmenin Temelleri</t>
+          <t>Mikroişlemci Sistemleri</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1809,22 +2337,22 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>afi, dersllik</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Akşam (14:00-15:15)</t>
+          <t>12:00-14:00</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Biyoinformatiğe Giriş</t>
+          <t xml:space="preserve">Yazılım Laboratuvarı I </t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1839,28 +2367,538 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>amfilerden biri</t>
+          <t>enes, adsas</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Sabah (09:00-10:15)</t>
+          <t>12:00-14:00</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
+          <t>Staj II</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>100</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>75 dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>oooo, mmmm</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>12:00-14:00</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Bilgi Güvenliği ve Kriptografi</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>100</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>75 dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>ss, sdsdsd</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>12:00-14:00</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Robotlar için Matematik Temelleri</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>100</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>75 dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>aa, fgfg</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>12:00-14:00</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Araştırma Problemleri</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>100</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>75 dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>a, sd, a</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>12:00-14:00</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Bitirme Çalışması</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>100</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>75 dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>301, Büyük Amfi</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>14:00-16:00</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Bilgisayar Ağları</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>100</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>75 dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>303, EDA</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>14:00-16:00</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>İş Hayatı ve İş Güvenliğine Hazırlık</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>100</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>75 dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>305, 400</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>14:00-16:00</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Programlanabilir Yapılar</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>100</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>75 dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>amfimsi, küçük amfi</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>14:00-16:00</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Yazılım Proje Yönetimi</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>100</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>75 dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>100, 212</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>14:00-16:00</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Bilgisayarlı Görmenin Temelleri</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>100</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>75 dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Yazılım Amfi, Jeofizik Amfi</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>14:00-16:00</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Veri Madenciliğine Giriş</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>100</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>75 dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">amfilerden biri, HKAmsı </t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>14:00-16:00</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Mobil Programlama</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>100</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>75 dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>afi, dersllik</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>14:00-16:00</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Mühendisler için İstatistik</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>100</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>75 dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>enes, adsas</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>14:00-16:00</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Derin Öğrenmenin Temelleri</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>100</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>75 dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>oooo, mmmm</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>14:00-16:00</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Doğal Dil İşleme ve Metin Madenciliğine Giriş</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>100</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>75 dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>ss, sdsdsd</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>14:00-16:00</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Gezgin Robotlara Giriş</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>100</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>75 dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>aa, fgfg</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>14:00-16:00</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Biyoinformatiğe Giriş</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>100</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>75 dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>a, sd, a</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>14:00-16:00</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
           <t>Bilgisayar Semineri</t>
         </is>
       </c>
-      <c r="E23" t="n">
-        <v>100</v>
-      </c>
-      <c r="F23" t="inlineStr">
+      <c r="E40" t="n">
+        <v>100</v>
+      </c>
+      <c r="F40" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -1872,6 +2910,63 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tarih</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Sınav Sayısı</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Toplam Öğrenci</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Kullanılan Oda</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>39</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3900</v>
+      </c>
+      <c r="D2" t="n">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1917,7 +3012,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-09-29</t>
         </is>
       </c>
     </row>
@@ -1929,7 +3024,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-05</t>
         </is>
       </c>
     </row>
@@ -2001,7 +3096,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>39</t>
         </is>
       </c>
     </row>
@@ -2013,7 +3108,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>İşaret ve Sistemler, Mikroişlemci Sistemleri, Fizik I, Mantıksal Tasarım ve Uygulamalar, Staj I, İş Hayatı ve İş Güvenliğine Hazırlık, Doğal Dil İşleme ve Metin Madenciliğine Giriş, Programlama I , Programlama Laboratuvarı - I , Gezgin Robotlara Giriş, Bilgisayar Laboratuvarı I, İngilizce I, Bilgisayarlı Görmenin Temelleri, Robotlar için Matematik Temelleri, Araştırma Problemleri, Türk Dili I, Mühendisler için İstatistik</t>
+          <t>Yok</t>
         </is>
       </c>
     </row>
@@ -2022,7 +3117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
create exam program fix
</commit_message>
<xml_diff>
--- a/sinav_programi.xlsx
+++ b/sinav_programi.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,25 +450,35 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Sınıf</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Tarih</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Seans</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Başlangıç Saati</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Oda</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Öğrenci Sayısı</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Süre (dk)</t>
         </is>
@@ -487,579 +497,769 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>2025-09-29</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>301, Büyük Amfi</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>100</v>
-      </c>
-      <c r="G2" t="n">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>100</v>
+      </c>
+      <c r="I2" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TDB107</t>
+          <t>MUH445</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Türk Dili I</t>
+          <t>Mühendisler için İstatistik</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>2025-09-29</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>303, EDA</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>100</v>
-      </c>
-      <c r="G3" t="n">
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>100</v>
+      </c>
+      <c r="I3" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>YDB117</t>
+          <t>TDB107</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>İngilizce I</t>
+          <t>Türk Dili I</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-09-30</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>0</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>305, 400</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>100</v>
-      </c>
-      <c r="G4" t="n">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>100</v>
+      </c>
+      <c r="I4" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FEF111</t>
+          <t>FEF203</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Fizik I</t>
+          <t>Diferansiyel Denklemler</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>amfimsi, küçük amfi</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>100</v>
-      </c>
-      <c r="G5" t="n">
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-09-30</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>100</v>
+      </c>
+      <c r="I5" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>FEF113</t>
+          <t>BLM451</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Lineer Cebir</t>
+          <t>Derin Öğrenmenin Temelleri</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>100, 212</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>100</v>
-      </c>
-      <c r="G6" t="n">
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-09-30</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>100</v>
+      </c>
+      <c r="I6" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>FEF115</t>
+          <t>YDB117</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Matematik I</t>
+          <t>İngilizce I</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
         <v>0</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Yazılım Amfi, Jeofizik Amfi</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>100</v>
-      </c>
-      <c r="G7" t="n">
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>100</v>
+      </c>
+      <c r="I7" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BLM101</t>
+          <t>MUH201</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Bilgisayar Laboratuvarı I</t>
+          <t>Nesneye Yönelik Programlama</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">amfilerden biri, HKAmsı </t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>100</v>
-      </c>
-      <c r="G8" t="n">
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>100</v>
+      </c>
+      <c r="I8" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BLM103</t>
+          <t>MUH301</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Bilgisayar Mühendisliğine Giriş</t>
+          <t>Sayısal Yöntemler</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>afi, dersllik</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>100</v>
-      </c>
-      <c r="G9" t="n">
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>4</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>100</v>
+      </c>
+      <c r="I9" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BLM105</t>
+          <t>BLM443</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Programlama I </t>
+          <t>Doğal Dil İşleme ve Metin Madenciliğine Giriş</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>enes, adsas</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>100</v>
-      </c>
-      <c r="G10" t="n">
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>6</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>100</v>
+      </c>
+      <c r="I10" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>FEF203</t>
+          <t>FEF111</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Diferansiyel Denklemler</t>
+          <t>Fizik I</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
         <v>0</v>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>oooo, mmmm</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>100</v>
-      </c>
-      <c r="G11" t="n">
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>100</v>
+      </c>
+      <c r="I11" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MUH201</t>
+          <t>BLM207</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Nesneye Yönelik Programlama</t>
+          <t>Veri Yapıları ve Algoritmaları</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>ss, sdsdsd</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>100</v>
-      </c>
-      <c r="G12" t="n">
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>100</v>
+      </c>
+      <c r="I12" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BLM207</t>
+          <t>BLM303</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Veri Yapıları ve Algoritmaları</t>
+          <t>İşaret ve Sistemler</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>aa, fgfg</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>100</v>
-      </c>
-      <c r="G13" t="n">
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>4</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>100</v>
+      </c>
+      <c r="I13" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BLM209</t>
+          <t>MUH403</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Programlama Laboratuvarı - I </t>
+          <t>Araştırma Problemleri</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>a, sd, a</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
-        <v>100</v>
-      </c>
-      <c r="G14" t="n">
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>6</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>100</v>
+      </c>
+      <c r="I14" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>BLM211</t>
+          <t>FEF113</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Mantıksal Tasarım ve Uygulamalar</t>
+          <t>Lineer Cebir</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>301, Büyük Amfi</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
-        <v>100</v>
-      </c>
-      <c r="G15" t="n">
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>100</v>
+      </c>
+      <c r="I15" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>BLM205</t>
+          <t>BLM209</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Ayrık Matematik</t>
+          <t xml:space="preserve">Programlama Laboratuvarı - I </t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>303, EDA</t>
-        </is>
-      </c>
-      <c r="F16" t="n">
-        <v>100</v>
-      </c>
-      <c r="G16" t="n">
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>100</v>
+      </c>
+      <c r="I16" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>BLM213</t>
+          <t>BLM305</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Staj I</t>
+          <t>İşletim Sistemleri</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>305, 400</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
-        <v>100</v>
-      </c>
-      <c r="G17" t="n">
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>4</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>100</v>
+      </c>
+      <c r="I17" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>MUH301</t>
+          <t>MUH402</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Sayısal Yöntemler</t>
+          <t>Bitirme Çalışması</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>amfimsi, küçük amfi</t>
-        </is>
-      </c>
-      <c r="F18" t="n">
-        <v>100</v>
-      </c>
-      <c r="G18" t="n">
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>6</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>100</v>
+      </c>
+      <c r="I18" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BLM303</t>
+          <t>FEF115</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>İşaret ve Sistemler</t>
+          <t>Matematik I</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>1</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>100, 212</t>
-        </is>
-      </c>
-      <c r="F19" t="n">
-        <v>100</v>
-      </c>
-      <c r="G19" t="n">
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>100</v>
+      </c>
+      <c r="I19" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BLM305</t>
+          <t>BLM211</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>İşletim Sistemleri</t>
+          <t>Mantıksal Tasarım ve Uygulamalar</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>1</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Yazılım Amfi, Jeofizik Amfi</t>
-        </is>
-      </c>
-      <c r="F20" t="n">
-        <v>100</v>
-      </c>
-      <c r="G20" t="n">
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>100</v>
+      </c>
+      <c r="I20" t="n">
         <v>75</v>
       </c>
     </row>
@@ -1076,269 +1276,359 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">amfilerden biri, HKAmsı </t>
-        </is>
-      </c>
-      <c r="F21" t="n">
-        <v>100</v>
-      </c>
-      <c r="G21" t="n">
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>4</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>100</v>
+      </c>
+      <c r="I21" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>BLM307</t>
+          <t>BLM401</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yazılım Laboratuvarı I </t>
+          <t>Bilgisayar Ağları</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>1</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>afi, dersllik</t>
-        </is>
-      </c>
-      <c r="F22" t="n">
-        <v>100</v>
-      </c>
-      <c r="G22" t="n">
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>6</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>100</v>
+      </c>
+      <c r="I22" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>BLM309</t>
+          <t>BLM101</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Staj II</t>
+          <t>Bilgisayar Laboratuvarı I</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>enes, adsas</t>
-        </is>
-      </c>
-      <c r="F23" t="n">
-        <v>100</v>
-      </c>
-      <c r="G23" t="n">
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>100</v>
+      </c>
+      <c r="I23" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>BLM323</t>
+          <t>BLM205</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Bilgi Güvenliği ve Kriptografi</t>
+          <t>Ayrık Matematik</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>1</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>oooo, mmmm</t>
-        </is>
-      </c>
-      <c r="F24" t="n">
-        <v>100</v>
-      </c>
-      <c r="G24" t="n">
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>100</v>
+      </c>
+      <c r="I24" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>BLM321</t>
+          <t>BLM307</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Robotlar için Matematik Temelleri</t>
+          <t xml:space="preserve">Yazılım Laboratuvarı I </t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>1</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>ss, sdsdsd</t>
-        </is>
-      </c>
-      <c r="F25" t="n">
-        <v>100</v>
-      </c>
-      <c r="G25" t="n">
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>4</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>100</v>
+      </c>
+      <c r="I25" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MUH403</t>
+          <t>BLM405</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Araştırma Problemleri</t>
+          <t>İş Hayatı ve İş Güvenliğine Hazırlık</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>1</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>aa, fgfg</t>
-        </is>
-      </c>
-      <c r="F26" t="n">
-        <v>100</v>
-      </c>
-      <c r="G26" t="n">
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>6</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>100</v>
+      </c>
+      <c r="I26" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>MUH402</t>
+          <t>BLM103</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Bitirme Çalışması</t>
+          <t>Bilgisayar Mühendisliğine Giriş</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>a, sd, a</t>
-        </is>
-      </c>
-      <c r="F27" t="n">
-        <v>100</v>
-      </c>
-      <c r="G27" t="n">
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2025-10-06</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>100</v>
+      </c>
+      <c r="I27" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>BLM401</t>
+          <t>BLM213</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Bilgisayar Ağları</t>
+          <t>Staj I</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2025-10-06</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
         <v>2</v>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>301, Büyük Amfi</t>
-        </is>
-      </c>
-      <c r="F28" t="n">
-        <v>100</v>
-      </c>
-      <c r="G28" t="n">
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>100</v>
+      </c>
+      <c r="I28" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>BLM405</t>
+          <t>BLM309</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>İş Hayatı ve İş Güvenliğine Hazırlık</t>
+          <t>Staj II</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>2</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>303, EDA</t>
-        </is>
-      </c>
-      <c r="F29" t="n">
-        <v>100</v>
-      </c>
-      <c r="G29" t="n">
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2025-10-06</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>4</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>100</v>
+      </c>
+      <c r="I29" t="n">
         <v>75</v>
       </c>
     </row>
@@ -1355,331 +1645,318 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>2</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>305, 400</t>
-        </is>
-      </c>
-      <c r="F30" t="n">
-        <v>100</v>
-      </c>
-      <c r="G30" t="n">
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2025-10-06</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>6</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>100</v>
+      </c>
+      <c r="I30" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>BLM421</t>
+          <t>BLM105</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Yazılım Proje Yönetimi</t>
+          <t xml:space="preserve">Programlama I </t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>2</v>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>amfimsi, küçük amfi</t>
-        </is>
-      </c>
-      <c r="F31" t="n">
-        <v>100</v>
-      </c>
-      <c r="G31" t="n">
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>100</v>
+      </c>
+      <c r="I31" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>BLM449</t>
+          <t>BLM323</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Bilgisayarlı Görmenin Temelleri</t>
+          <t>Bilgi Güvenliği ve Kriptografi</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
         <v>2</v>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>100, 212</t>
-        </is>
-      </c>
-      <c r="F32" t="n">
-        <v>100</v>
-      </c>
-      <c r="G32" t="n">
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>100</v>
+      </c>
+      <c r="I32" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>BLM429</t>
+          <t>BLM421</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Veri Madenciliğine Giriş</t>
+          <t>Yazılım Proje Yönetimi</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>2</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Yazılım Amfi, Jeofizik Amfi</t>
-        </is>
-      </c>
-      <c r="F33" t="n">
-        <v>100</v>
-      </c>
-      <c r="G33" t="n">
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>4</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>100</v>
+      </c>
+      <c r="I33" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>BLM441</t>
+          <t>BLM321</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Mobil Programlama</t>
+          <t>Robotlar için Matematik Temelleri</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>2</v>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t xml:space="preserve">amfilerden biri, HKAmsı </t>
-        </is>
-      </c>
-      <c r="F34" t="n">
-        <v>100</v>
-      </c>
-      <c r="G34" t="n">
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2025-10-08</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>100</v>
+      </c>
+      <c r="I34" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>MUH445</t>
+          <t>BLM449</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Mühendisler için İstatistik</t>
+          <t>Bilgisayarlı Görmenin Temelleri</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2025-10-08</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
         <v>2</v>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>afi, dersllik</t>
-        </is>
-      </c>
-      <c r="F35" t="n">
-        <v>100</v>
-      </c>
-      <c r="G35" t="n">
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>100</v>
+      </c>
+      <c r="I35" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>BLM451</t>
+          <t>BLM429</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Derin Öğrenmenin Temelleri</t>
+          <t>Veri Madenciliğine Giriş</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>2</v>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>enes, adsas</t>
-        </is>
-      </c>
-      <c r="F36" t="n">
-        <v>100</v>
-      </c>
-      <c r="G36" t="n">
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2025-10-09</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>100</v>
+      </c>
+      <c r="I36" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>BLM443</t>
+          <t>BLM441</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Doğal Dil İşleme ve Metin Madenciliğine Giriş</t>
+          <t>Mobil Programlama</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>2</v>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>oooo, mmmm</t>
-        </is>
-      </c>
-      <c r="F37" t="n">
-        <v>100</v>
-      </c>
-      <c r="G37" t="n">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>MUH413</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Gezgin Robotlara Giriş</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
-        <v>2</v>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>ss, sdsdsd</t>
-        </is>
-      </c>
-      <c r="F38" t="n">
-        <v>100</v>
-      </c>
-      <c r="G38" t="n">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>BLM435</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Biyoinformatiğe Giriş</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D39" t="n">
-        <v>2</v>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>aa, fgfg</t>
-        </is>
-      </c>
-      <c r="F39" t="n">
-        <v>100</v>
-      </c>
-      <c r="G39" t="n">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>BLM411</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Bilgisayar Semineri</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="D40" t="n">
-        <v>2</v>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>a, sd, a</t>
-        </is>
-      </c>
-      <c r="F40" t="n">
-        <v>100</v>
-      </c>
-      <c r="G40" t="n">
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2025-10-10</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>EDA, HKA, 301</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>100</v>
+      </c>
+      <c r="I37" t="n">
         <v>75</v>
       </c>
     </row>
@@ -1694,7 +1971,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1725,10 +2002,15 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Sınıf</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Öğrenci</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Süre</t>
         </is>
@@ -1737,7 +2019,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>301, Büyük Amfi</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1755,10 +2037,15 @@
           <t>Atatürk İlkeleri ve İnkılap Tarihi I</t>
         </is>
       </c>
-      <c r="E2" t="n">
-        <v>100</v>
-      </c>
-      <c r="F2" t="inlineStr">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -1767,12 +2054,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>303, EDA</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1785,10 +2072,15 @@
           <t>Türk Dili I</t>
         </is>
       </c>
-      <c r="E3" t="n">
-        <v>100</v>
-      </c>
-      <c r="F3" t="inlineStr">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>100</v>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -1797,12 +2089,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>305, 400</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1815,10 +2107,15 @@
           <t>İngilizce I</t>
         </is>
       </c>
-      <c r="E4" t="n">
-        <v>100</v>
-      </c>
-      <c r="F4" t="inlineStr">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>100</v>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -1827,12 +2124,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>amfimsi, küçük amfi</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1845,10 +2142,15 @@
           <t>Fizik I</t>
         </is>
       </c>
-      <c r="E5" t="n">
-        <v>100</v>
-      </c>
-      <c r="F5" t="inlineStr">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>100</v>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -1857,12 +2159,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>100, 212</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1875,10 +2177,15 @@
           <t>Lineer Cebir</t>
         </is>
       </c>
-      <c r="E6" t="n">
-        <v>100</v>
-      </c>
-      <c r="F6" t="inlineStr">
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>100</v>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -1887,12 +2194,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Yazılım Amfi, Jeofizik Amfi</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1905,10 +2212,15 @@
           <t>Matematik I</t>
         </is>
       </c>
-      <c r="E7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F7" t="inlineStr">
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>100</v>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -1917,12 +2229,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">amfilerden biri, HKAmsı </t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-05</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1935,10 +2247,15 @@
           <t>Bilgisayar Laboratuvarı I</t>
         </is>
       </c>
-      <c r="E8" t="n">
-        <v>100</v>
-      </c>
-      <c r="F8" t="inlineStr">
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>100</v>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -1947,12 +2264,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>afi, dersllik</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-06</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1965,10 +2282,15 @@
           <t>Bilgisayar Mühendisliğine Giriş</t>
         </is>
       </c>
-      <c r="E9" t="n">
-        <v>100</v>
-      </c>
-      <c r="F9" t="inlineStr">
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>100</v>
+      </c>
+      <c r="G9" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -1977,12 +2299,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>enes, adsas</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-07</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1995,10 +2317,15 @@
           <t xml:space="preserve">Programlama I </t>
         </is>
       </c>
-      <c r="E10" t="n">
-        <v>100</v>
-      </c>
-      <c r="F10" t="inlineStr">
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>100</v>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2007,17 +2334,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>oooo, mmmm</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>10:00-12:00</t>
+          <t>14:00-16:00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -2025,10 +2352,15 @@
           <t>Diferansiyel Denklemler</t>
         </is>
       </c>
-      <c r="E11" t="n">
-        <v>100</v>
-      </c>
-      <c r="F11" t="inlineStr">
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>100</v>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2037,17 +2369,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ss, sdsdsd</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>10:00-12:00</t>
+          <t>14:00-16:00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -2055,10 +2387,15 @@
           <t>Nesneye Yönelik Programlama</t>
         </is>
       </c>
-      <c r="E12" t="n">
-        <v>100</v>
-      </c>
-      <c r="F12" t="inlineStr">
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>100</v>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2067,17 +2404,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>aa, fgfg</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>10:00-12:00</t>
+          <t>14:00-16:00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -2085,10 +2422,15 @@
           <t>Veri Yapıları ve Algoritmaları</t>
         </is>
       </c>
-      <c r="E13" t="n">
-        <v>100</v>
-      </c>
-      <c r="F13" t="inlineStr">
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>100</v>
+      </c>
+      <c r="G13" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2097,17 +2439,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>a, sd, a</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>10:00-12:00</t>
+          <t>14:00-16:00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -2115,10 +2457,15 @@
           <t xml:space="preserve">Programlama Laboratuvarı - I </t>
         </is>
       </c>
-      <c r="E14" t="n">
-        <v>100</v>
-      </c>
-      <c r="F14" t="inlineStr">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>100</v>
+      </c>
+      <c r="G14" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2127,17 +2474,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>301, Büyük Amfi</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>12:00-14:00</t>
+          <t>14:00-16:00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -2145,10 +2492,15 @@
           <t>Mantıksal Tasarım ve Uygulamalar</t>
         </is>
       </c>
-      <c r="E15" t="n">
-        <v>100</v>
-      </c>
-      <c r="F15" t="inlineStr">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>100</v>
+      </c>
+      <c r="G15" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2157,17 +2509,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>303, EDA</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-05</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>12:00-14:00</t>
+          <t>14:00-16:00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -2175,10 +2527,15 @@
           <t>Ayrık Matematik</t>
         </is>
       </c>
-      <c r="E16" t="n">
-        <v>100</v>
-      </c>
-      <c r="F16" t="inlineStr">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>100</v>
+      </c>
+      <c r="G16" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2187,17 +2544,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>305, 400</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-06</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>12:00-14:00</t>
+          <t>14:00-16:00</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -2205,10 +2562,15 @@
           <t>Staj I</t>
         </is>
       </c>
-      <c r="E17" t="n">
-        <v>100</v>
-      </c>
-      <c r="F17" t="inlineStr">
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>100</v>
+      </c>
+      <c r="G17" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2217,17 +2579,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>amfimsi, küçük amfi</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>12:00-14:00</t>
+          <t>18:00-20:00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -2235,10 +2597,15 @@
           <t>Sayısal Yöntemler</t>
         </is>
       </c>
-      <c r="E18" t="n">
-        <v>100</v>
-      </c>
-      <c r="F18" t="inlineStr">
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>100</v>
+      </c>
+      <c r="G18" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2247,17 +2614,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>100, 212</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>12:00-14:00</t>
+          <t>18:00-20:00</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -2265,10 +2632,15 @@
           <t>İşaret ve Sistemler</t>
         </is>
       </c>
-      <c r="E19" t="n">
-        <v>100</v>
-      </c>
-      <c r="F19" t="inlineStr">
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>100</v>
+      </c>
+      <c r="G19" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2277,17 +2649,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Yazılım Amfi, Jeofizik Amfi</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>12:00-14:00</t>
+          <t>18:00-20:00</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -2295,10 +2667,15 @@
           <t>İşletim Sistemleri</t>
         </is>
       </c>
-      <c r="E20" t="n">
-        <v>100</v>
-      </c>
-      <c r="F20" t="inlineStr">
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>100</v>
+      </c>
+      <c r="G20" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2307,17 +2684,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve">amfilerden biri, HKAmsı </t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>12:00-14:00</t>
+          <t>18:00-20:00</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -2325,10 +2702,15 @@
           <t>Mikroişlemci Sistemleri</t>
         </is>
       </c>
-      <c r="E21" t="n">
-        <v>100</v>
-      </c>
-      <c r="F21" t="inlineStr">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>100</v>
+      </c>
+      <c r="G21" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2337,17 +2719,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>afi, dersllik</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-05</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>12:00-14:00</t>
+          <t>18:00-20:00</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2355,10 +2737,15 @@
           <t xml:space="preserve">Yazılım Laboratuvarı I </t>
         </is>
       </c>
-      <c r="E22" t="n">
-        <v>100</v>
-      </c>
-      <c r="F22" t="inlineStr">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>100</v>
+      </c>
+      <c r="G22" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2367,17 +2754,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>enes, adsas</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-06</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>12:00-14:00</t>
+          <t>18:00-20:00</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2385,10 +2772,15 @@
           <t>Staj II</t>
         </is>
       </c>
-      <c r="E23" t="n">
-        <v>100</v>
-      </c>
-      <c r="F23" t="inlineStr">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>100</v>
+      </c>
+      <c r="G23" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2397,17 +2789,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>oooo, mmmm</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-07</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>12:00-14:00</t>
+          <t>14:00-16:00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2415,10 +2807,15 @@
           <t>Bilgi Güvenliği ve Kriptografi</t>
         </is>
       </c>
-      <c r="E24" t="n">
-        <v>100</v>
-      </c>
-      <c r="F24" t="inlineStr">
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>100</v>
+      </c>
+      <c r="G24" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2427,17 +2824,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>ss, sdsdsd</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>12:00-14:00</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2445,10 +2842,15 @@
           <t>Robotlar için Matematik Temelleri</t>
         </is>
       </c>
-      <c r="E25" t="n">
-        <v>100</v>
-      </c>
-      <c r="F25" t="inlineStr">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>100</v>
+      </c>
+      <c r="G25" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2457,17 +2859,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>aa, fgfg</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>12:00-14:00</t>
+          <t>Slot 7</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2475,10 +2877,15 @@
           <t>Araştırma Problemleri</t>
         </is>
       </c>
-      <c r="E26" t="n">
-        <v>100</v>
-      </c>
-      <c r="F26" t="inlineStr">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>100</v>
+      </c>
+      <c r="G26" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2487,17 +2894,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>a, sd, a</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>12:00-14:00</t>
+          <t>Slot 7</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2505,10 +2912,15 @@
           <t>Bitirme Çalışması</t>
         </is>
       </c>
-      <c r="E27" t="n">
-        <v>100</v>
-      </c>
-      <c r="F27" t="inlineStr">
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>100</v>
+      </c>
+      <c r="G27" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2517,17 +2929,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>301, Büyük Amfi</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>14:00-16:00</t>
+          <t>Slot 7</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2535,10 +2947,15 @@
           <t>Bilgisayar Ağları</t>
         </is>
       </c>
-      <c r="E28" t="n">
-        <v>100</v>
-      </c>
-      <c r="F28" t="inlineStr">
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>100</v>
+      </c>
+      <c r="G28" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2547,17 +2964,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>303, EDA</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-05</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>14:00-16:00</t>
+          <t>Slot 7</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2565,10 +2982,15 @@
           <t>İş Hayatı ve İş Güvenliğine Hazırlık</t>
         </is>
       </c>
-      <c r="E29" t="n">
-        <v>100</v>
-      </c>
-      <c r="F29" t="inlineStr">
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>100</v>
+      </c>
+      <c r="G29" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2577,17 +2999,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>305, 400</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-06</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>14:00-16:00</t>
+          <t>Slot 7</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2595,10 +3017,15 @@
           <t>Programlanabilir Yapılar</t>
         </is>
       </c>
-      <c r="E30" t="n">
-        <v>100</v>
-      </c>
-      <c r="F30" t="inlineStr">
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>100</v>
+      </c>
+      <c r="G30" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2607,17 +3034,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>amfimsi, küçük amfi</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-07</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>14:00-16:00</t>
+          <t>18:00-20:00</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2625,10 +3052,15 @@
           <t>Yazılım Proje Yönetimi</t>
         </is>
       </c>
-      <c r="E31" t="n">
-        <v>100</v>
-      </c>
-      <c r="F31" t="inlineStr">
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>100</v>
+      </c>
+      <c r="G31" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2637,12 +3069,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>100, 212</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2655,10 +3087,15 @@
           <t>Bilgisayarlı Görmenin Temelleri</t>
         </is>
       </c>
-      <c r="E32" t="n">
-        <v>100</v>
-      </c>
-      <c r="F32" t="inlineStr">
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>100</v>
+      </c>
+      <c r="G32" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2667,17 +3104,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Yazılım Amfi, Jeofizik Amfi</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-09</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>14:00-16:00</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2685,10 +3122,15 @@
           <t>Veri Madenciliğine Giriş</t>
         </is>
       </c>
-      <c r="E33" t="n">
-        <v>100</v>
-      </c>
-      <c r="F33" t="inlineStr">
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>100</v>
+      </c>
+      <c r="G33" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2697,17 +3139,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t xml:space="preserve">amfilerden biri, HKAmsı </t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-10</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>14:00-16:00</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2715,10 +3157,15 @@
           <t>Mobil Programlama</t>
         </is>
       </c>
-      <c r="E34" t="n">
-        <v>100</v>
-      </c>
-      <c r="F34" t="inlineStr">
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>100</v>
+      </c>
+      <c r="G34" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2727,7 +3174,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>afi, dersllik</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2745,10 +3192,15 @@
           <t>Mühendisler için İstatistik</t>
         </is>
       </c>
-      <c r="E35" t="n">
-        <v>100</v>
-      </c>
-      <c r="F35" t="inlineStr">
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>100</v>
+      </c>
+      <c r="G35" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2757,17 +3209,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>enes, adsas</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>14:00-16:00</t>
+          <t>18:00-20:00</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -2775,10 +3227,15 @@
           <t>Derin Öğrenmenin Temelleri</t>
         </is>
       </c>
-      <c r="E36" t="n">
-        <v>100</v>
-      </c>
-      <c r="F36" t="inlineStr">
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>100</v>
+      </c>
+      <c r="G36" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2787,17 +3244,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>oooo, mmmm</t>
+          <t>EDA, HKA, 301</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>14:00-16:00</t>
+          <t>Slot 7</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -2805,100 +3262,15 @@
           <t>Doğal Dil İşleme ve Metin Madenciliğine Giriş</t>
         </is>
       </c>
-      <c r="E37" t="n">
-        <v>100</v>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>75 dk</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>ss, sdsdsd</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>14:00-16:00</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Gezgin Robotlara Giriş</t>
-        </is>
-      </c>
-      <c r="E38" t="n">
-        <v>100</v>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>75 dk</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>aa, fgfg</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>14:00-16:00</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Biyoinformatiğe Giriş</t>
-        </is>
-      </c>
-      <c r="E39" t="n">
-        <v>100</v>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>75 dk</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>a, sd, a</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>2025-09-29</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>14:00-16:00</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Bilgisayar Semineri</t>
-        </is>
-      </c>
-      <c r="E40" t="n">
-        <v>100</v>
-      </c>
-      <c r="F40" t="inlineStr">
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>100</v>
+      </c>
+      <c r="G37" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2915,7 +3287,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2952,13 +3324,189 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>3900</v>
+        <v>200</v>
       </c>
       <c r="D2" t="n">
-        <v>27</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-09-30</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>300</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" t="n">
+        <v>400</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="n">
+        <v>400</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>400</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" t="n">
+        <v>400</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" t="n">
+        <v>400</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-10-06</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" t="n">
+        <v>400</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" t="n">
+        <v>300</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-10-08</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" t="n">
+        <v>200</v>
+      </c>
+      <c r="D11" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-10-09</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>100</v>
+      </c>
+      <c r="D12" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-10-10</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>100</v>
+      </c>
+      <c r="D13" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3024,7 +3572,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-10-05</t>
+          <t>2025-10-10</t>
         </is>
       </c>
     </row>
@@ -3079,12 +3627,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Çakışma Kontrolü</t>
+          <t>Farklı Sınıflar Aynı Anda</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Aktif</t>
+          <t>İzin Verilir</t>
         </is>
       </c>
     </row>
@@ -3096,7 +3644,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>36</t>
         </is>
       </c>
     </row>
@@ -3123,7 +3671,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3141,7 +3689,49 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>✅ Uyarı yok</t>
+          <t>❌ 'Gezgin Robotlara Giriş' yerleştirilemedi (Öğrenci: 100, Sınıf: 4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>❌ 'Biyoinformatiğe Giriş' yerleştirilemedi (Öğrenci: 100, Sınıf: 4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>❌ 'Bilgisayar Semineri' yerleştirilemedi (Öğrenci: 100, Sınıf: 4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>⚠️ 3 ders yerleştirilemedi!</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • Gezgin Robotlara Giriş (Öğrenci: 100, Yıl: 4, Süre: 75 dk)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • Biyoinformatiğe Giriş (Öğrenci: 100, Yıl: 4, Süre: 75 dk)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   • Bilgisayar Semineri (Öğrenci: 100, Yıl: 4, Süre: 75 dk)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
restart to exam program.
</commit_message>
<xml_diff>
--- a/sinav_programi.xlsx
+++ b/sinav_programi.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,7 +515,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -556,7 +556,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -569,12 +569,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MUH301</t>
+          <t>BLM303</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Sayısal Yöntemler</t>
+          <t>İşaret ve Sistemler</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -597,7 +597,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -610,12 +610,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MUH403</t>
+          <t>MUH413</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Araştırma Problemleri</t>
+          <t>Gezgin Robotlara Giriş</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -629,16 +629,16 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -651,17 +651,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BLM101</t>
+          <t>MUH403</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Bilgisayar Laboratuvarı I</t>
+          <t>Araştırma Problemleri</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -670,16 +670,16 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -720,7 +720,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -761,7 +761,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -774,12 +774,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BLM303</t>
+          <t>BLM325</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>İşaret ve Sistemler</t>
+          <t>Mikroişlemci Sistemleri</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -802,7 +802,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -843,7 +843,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -856,12 +856,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BLM103</t>
+          <t>FEF111</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Bilgisayar Mühendisliğine Giriş</t>
+          <t>Fizik I</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -871,20 +871,20 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -897,17 +897,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>YDB117</t>
+          <t>BLM209</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>İngilizce I</t>
+          <t xml:space="preserve">Programlama Laboratuvarı - I </t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -916,16 +916,16 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -938,17 +938,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BLM207</t>
+          <t>BLM307</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Veri Yapıları ve Algoritmaları</t>
+          <t xml:space="preserve">Yazılım Laboratuvarı I </t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -957,16 +957,16 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -979,17 +979,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BLM305</t>
+          <t>BLM401</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>İşletim Sistemleri</t>
+          <t>Bilgisayar Ağları</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -1020,35 +1020,35 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>BLM401</t>
+          <t>FEF113</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Bilgisayar Ağları</t>
+          <t>Lineer Cebir</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -1061,35 +1061,35 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>BLM105</t>
+          <t>BLM205</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Programlama I </t>
+          <t>Ayrık Matematik</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -1102,17 +1102,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>FEF111</t>
+          <t>BLM323</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Fizik I</t>
+          <t>Bilgi Güvenliği ve Kriptografi</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1121,16 +1121,16 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -1143,17 +1143,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>BLM209</t>
+          <t>BLM417</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Programlama Laboratuvarı - I </t>
+          <t>Programlanabilir Yapılar</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1162,16 +1162,16 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H18" t="n">
@@ -1184,35 +1184,35 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BLM325</t>
+          <t>BLM101</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Mikroişlemci Sistemleri</t>
+          <t>Bilgisayar Laboratuvarı I</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -1225,35 +1225,35 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BLM405</t>
+          <t>BLM213</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>İş Hayatı ve İş Güvenliğine Hazırlık</t>
+          <t>Staj I</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H20" t="n">
@@ -1266,35 +1266,35 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>BLM213</t>
+          <t>BLM449</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Staj I</t>
+          <t>Bilgisayarlı Görmenin Temelleri</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H21" t="n">
@@ -1307,12 +1307,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>FEF113</t>
+          <t>BLM105</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Lineer Cebir</t>
+          <t xml:space="preserve">Programlama I </t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1322,7 +1322,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1335,7 +1335,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -1348,22 +1348,22 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>BLM211</t>
+          <t>BLM441</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Mantıksal Tasarım ve Uygulamalar</t>
+          <t>Mobil Programlama</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -1376,7 +1376,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H23" t="n">
@@ -1389,35 +1389,35 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>BLM307</t>
+          <t>MUH445</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yazılım Laboratuvarı I </t>
+          <t>Mühendisler için İstatistik</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-05</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H24" t="n">
@@ -1430,12 +1430,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>BLM417</t>
+          <t>BLM443</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Programlanabilir Yapılar</t>
+          <t>Doğal Dil İşleme ve Metin Madenciliğine Giriş</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1445,20 +1445,20 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-06</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H25" t="n">
@@ -1471,246 +1471,41 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>BLM323</t>
+          <t>BLM411</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Bilgi Güvenliği ve Kriptografi</t>
+          <t>Bilgisayar Semineri</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-06</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="H26" t="n">
         <v>100</v>
       </c>
       <c r="I26" t="n">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>FEF115</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Matematik I</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>2025-10-04</t>
-        </is>
-      </c>
-      <c r="E27" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>a, EDA, Büyük Amfi</t>
-        </is>
-      </c>
-      <c r="H27" t="n">
-        <v>100</v>
-      </c>
-      <c r="I27" t="n">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>BLM205</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Ayrık Matematik</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>2025-10-04</t>
-        </is>
-      </c>
-      <c r="E28" t="n">
-        <v>2</v>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>a, EDA, Büyük Amfi</t>
-        </is>
-      </c>
-      <c r="H28" t="n">
-        <v>100</v>
-      </c>
-      <c r="I28" t="n">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>BLM309</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Staj II</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>2025-10-04</t>
-        </is>
-      </c>
-      <c r="E29" t="n">
-        <v>4</v>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>a, EDA, Büyük Amfi</t>
-        </is>
-      </c>
-      <c r="H29" t="n">
-        <v>100</v>
-      </c>
-      <c r="I29" t="n">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>BLM421</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Yazılım Proje Yönetimi</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>2025-10-04</t>
-        </is>
-      </c>
-      <c r="E30" t="n">
-        <v>6</v>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>a, EDA, Büyük Amfi</t>
-        </is>
-      </c>
-      <c r="H30" t="n">
-        <v>100</v>
-      </c>
-      <c r="I30" t="n">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>BLM321</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Robotlar için Matematik Temelleri</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>2025-10-04</t>
-        </is>
-      </c>
-      <c r="E31" t="n">
-        <v>8</v>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>a, EDA, Büyük Amfi</t>
-        </is>
-      </c>
-      <c r="H31" t="n">
-        <v>100</v>
-      </c>
-      <c r="I31" t="n">
         <v>75</v>
       </c>
     </row>
@@ -1725,7 +1520,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1773,7 +1568,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1808,7 +1603,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1843,7 +1638,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1858,7 +1653,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>İngilizce I</t>
+          <t>Fizik I</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1878,7 +1673,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1893,7 +1688,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Fizik I</t>
+          <t>Lineer Cebir</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1913,7 +1708,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1928,7 +1723,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Lineer Cebir</t>
+          <t>Bilgisayar Laboratuvarı I</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1948,7 +1743,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1963,7 +1758,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Matematik I</t>
+          <t xml:space="preserve">Programlama I </t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1983,7 +1778,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2018,7 +1813,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2053,7 +1848,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2068,7 +1863,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Veri Yapıları ve Algoritmaları</t>
+          <t xml:space="preserve">Programlama Laboratuvarı - I </t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -2088,7 +1883,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2103,7 +1898,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Programlama Laboratuvarı - I </t>
+          <t>Ayrık Matematik</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -2123,7 +1918,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2138,7 +1933,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Mantıksal Tasarım ve Uygulamalar</t>
+          <t>Staj I</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -2158,27 +1953,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>14:00-16:00</t>
+          <t>18:00-20:00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Ayrık Matematik</t>
+          <t>İşaret ve Sistemler</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -2193,12 +1988,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -2208,7 +2003,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Sayısal Yöntemler</t>
+          <t>Mikroişlemci Sistemleri</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -2228,12 +2023,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -2243,7 +2038,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>İşaret ve Sistemler</t>
+          <t xml:space="preserve">Yazılım Laboratuvarı I </t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -2263,12 +2058,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -2278,7 +2073,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>İşletim Sistemleri</t>
+          <t>Bilgi Güvenliği ve Kriptografi</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -2298,27 +2093,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>18:00-20:00</t>
+          <t>Slot 7</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Mikroişlemci Sistemleri</t>
+          <t>Araştırma Problemleri</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -2333,27 +2128,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>18:00-20:00</t>
+          <t>Slot 7</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yazılım Laboratuvarı I </t>
+          <t>Bitirme Çalışması</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -2368,27 +2163,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>18:00-20:00</t>
+          <t>Slot 7</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Staj II</t>
+          <t>Bilgisayar Ağları</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -2403,12 +2198,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2418,7 +2213,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Araştırma Problemleri</t>
+          <t>Programlanabilir Yapılar</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -2438,22 +2233,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Slot 7</t>
+          <t>18:00-20:00</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Bitirme Çalışması</t>
+          <t>Bilgisayarlı Görmenin Temelleri</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -2473,22 +2268,22 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Slot 7</t>
+          <t>14:00-16:00</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Bilgisayar Ağları</t>
+          <t>Mobil Programlama</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -2508,22 +2303,22 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-05</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Slot 7</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>İş Hayatı ve İş Güvenliğine Hazırlık</t>
+          <t>Mühendisler için İstatistik</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -2543,22 +2338,22 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-06</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Slot 7</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Programlanabilir Yapılar</t>
+          <t>Doğal Dil İşleme ve Metin Madenciliğine Giriş</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -2578,22 +2373,22 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Slot 7</t>
+          <t>18:00-20:00</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Yazılım Proje Yönetimi</t>
+          <t>Gezgin Robotlara Giriş</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -2613,208 +2408,33 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>a, EDA, Büyük Amfi</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-06</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Slot 9</t>
+          <t>Slot 10</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Bilgisayar Laboratuvarı I</t>
+          <t>Bilgisayar Semineri</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F26" t="n">
         <v>100</v>
       </c>
       <c r="G26" t="inlineStr">
-        <is>
-          <t>75 dk</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>a, EDA, Büyük Amfi</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Slot 9</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Bilgisayar Mühendisliğine Giriş</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F27" t="n">
-        <v>100</v>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>75 dk</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>a, EDA, Büyük Amfi</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>2025-10-01</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Slot 9</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Programlama I </t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F28" t="n">
-        <v>100</v>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>75 dk</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>a, EDA, Büyük Amfi</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>2025-10-02</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Slot 9</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Staj I</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="F29" t="n">
-        <v>100</v>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>75 dk</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>a, EDA, Büyük Amfi</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>2025-10-03</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Slot 9</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Bilgi Güvenliği ve Kriptografi</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="F30" t="n">
-        <v>100</v>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>75 dk</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>a, EDA, Büyük Amfi</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>2025-10-04</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Slot 9</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Robotlar için Matematik Temelleri</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="F31" t="n">
-        <v>100</v>
-      </c>
-      <c r="G31" t="inlineStr">
         <is>
           <t>75 dk</t>
         </is>
@@ -2831,7 +2451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2874,7 +2494,7 @@
         <v>500</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -2884,13 +2504,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -2900,13 +2520,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -2916,13 +2536,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -2932,13 +2552,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -2948,13 +2568,45 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>100</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-10-06</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>200</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3020,7 +2672,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-06</t>
         </is>
       </c>
     </row>
@@ -3075,7 +2727,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Farklı Sınıflar Aynı Anda</t>
+          <t>Aynı Seansta Çoklu Sınav</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -3092,7 +2744,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>25</t>
         </is>
       </c>
     </row>
@@ -3104,7 +2756,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Yok</t>
+          <t>Staj II, Mantıksal Tasarım ve Uygulamalar, İşletim Sistemleri, Veri Yapıları ve Algoritmaları, Bilgisayar Mühendisliğine Giriş, Sayısal Yöntemler, Biyoinformatiğe Giriş, Yazılım Proje Yönetimi, Matematik I, Veri Madenciliğine Giriş, İş Hayatı ve İş Güvenliğine Hazırlık, Robotlar için Matematik Temelleri, İngilizce I, Derin Öğrenmenin Temelleri</t>
         </is>
       </c>
     </row>
@@ -3119,7 +2771,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3137,105 +2789,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>❌ 'Bilgisayarlı Görmenin Temelleri' yerleştirilemedi (Öğrenci: 100, Sınıf: 4)</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>❌ 'Veri Madenciliğine Giriş' yerleştirilemedi (Öğrenci: 100, Sınıf: 4)</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>❌ 'Mobil Programlama' yerleştirilemedi (Öğrenci: 100, Sınıf: 4)</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>❌ 'Mühendisler için İstatistik' yerleştirilemedi (Öğrenci: 100, Sınıf: 4)</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>❌ 'Derin Öğrenmenin Temelleri' yerleştirilemedi (Öğrenci: 100, Sınıf: 4)</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>❌ 'Doğal Dil İşleme ve Metin Madenciliğine Giriş' yerleştirilemedi (Öğrenci: 100, Sınıf: 4)</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>❌ 'Gezgin Robotlara Giriş' yerleştirilemedi (Öğrenci: 100, Sınıf: 4)</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>❌ 'Biyoinformatiğe Giriş' yerleştirilemedi (Öğrenci: 100, Sınıf: 4)</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>❌ 'Bilgisayar Semineri' yerleştirilemedi (Öğrenci: 100, Sınıf: 4)</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>⚠️ 9 ders yerleştirilemedi!</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   • Bilgisayarlı Görmenin Temelleri (Öğrenci: 100, Yıl: 4, Süre: 75 dk)</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   • Veri Madenciliğine Giriş (Öğrenci: 100, Yıl: 4, Süre: 75 dk)</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   • Mobil Programlama (Öğrenci: 100, Yıl: 4, Süre: 75 dk)</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   • Mühendisler için İstatistik (Öğrenci: 100, Yıl: 4, Süre: 75 dk)</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   • Derin Öğrenmenin Temelleri (Öğrenci: 100, Yıl: 4, Süre: 75 dk)</t>
+          <t>✅ Uyarı yok</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
exam program fixes.Error handling.
</commit_message>
<xml_diff>
--- a/sinav_programi.xlsx
+++ b/sinav_programi.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="86">
   <si>
     <t>2025-09-29</t>
   </si>
@@ -37,9 +37,6 @@
     <t>2025-10-05</t>
   </si>
   <si>
-    <t>2025-10-06</t>
-  </si>
-  <si>
     <t>09:00</t>
   </si>
   <si>
@@ -55,202 +52,208 @@
     <t>15:00</t>
   </si>
   <si>
+    <t>16:30</t>
+  </si>
+  <si>
+    <t>18:00</t>
+  </si>
+  <si>
+    <t>Robotlar için Matematik Temelleri</t>
+  </si>
+  <si>
+    <t>Mikroişlemci Sistemleri</t>
+  </si>
+  <si>
+    <t>Ayrık Matematik</t>
+  </si>
+  <si>
+    <t>Bilgisayar Ağları</t>
+  </si>
+  <si>
+    <t>Doğal Dil İşleme ve Metin Madenciliğine Giriş</t>
+  </si>
+  <si>
+    <t>Araştırma Problemleri</t>
+  </si>
+  <si>
+    <t>Veri Madenciliğine Giriş</t>
+  </si>
+  <si>
+    <t>Sayısal Yöntemler</t>
+  </si>
+  <si>
+    <t>Matematik I</t>
+  </si>
+  <si>
+    <t>Staj II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programlama I </t>
+  </si>
+  <si>
+    <t>Diferansiyel Denklemler</t>
+  </si>
+  <si>
+    <t>Veri Yapıları ve Algoritmaları</t>
+  </si>
+  <si>
+    <t>Fizik I</t>
+  </si>
+  <si>
+    <t>Mühendisler için İstatistik</t>
+  </si>
+  <si>
+    <t>İşaret ve Sistemler</t>
+  </si>
+  <si>
+    <t>İş Hayatı ve İş Güvenliğine Hazırlık</t>
+  </si>
+  <si>
+    <t>İngilizce I</t>
+  </si>
+  <si>
     <t>Lineer Cebir</t>
   </si>
   <si>
+    <t xml:space="preserve">Programlama Laboratuvarı - I </t>
+  </si>
+  <si>
+    <t>Bitirme Çalışması</t>
+  </si>
+  <si>
+    <t>Yazılım Proje Yönetimi</t>
+  </si>
+  <si>
+    <t>Türk Dili I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yazılım Laboratuvarı I </t>
+  </si>
+  <si>
+    <t>Bilgisayar Laboratuvarı I</t>
+  </si>
+  <si>
+    <t>Bilgi Güvenliği ve Kriptografi</t>
+  </si>
+  <si>
+    <t>Biyoinformatiğe Giriş</t>
+  </si>
+  <si>
+    <t>Bilgisayar Semineri</t>
+  </si>
+  <si>
+    <t>Mobil Programlama</t>
+  </si>
+  <si>
     <t>Nesneye Yönelik Programlama</t>
   </si>
   <si>
-    <t>Bilgi Güvenliği ve Kriptografi</t>
+    <t>İşletim Sistemleri</t>
+  </si>
+  <si>
+    <t>Bilgisayarlı Görmenin Temelleri</t>
+  </si>
+  <si>
+    <t>Bilgisayar Mühendisliğine Giriş</t>
+  </si>
+  <si>
+    <t>Atatürk İlkeleri ve İnkılap Tarihi I</t>
+  </si>
+  <si>
+    <t>Derin Öğrenmenin Temelleri</t>
+  </si>
+  <si>
+    <t>Staj I</t>
   </si>
   <si>
     <t>Programlanabilir Yapılar</t>
   </si>
   <si>
-    <t>Bilgisayar Mühendisliğine Giriş</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Programlama Laboratuvarı - I </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yazılım Laboratuvarı I </t>
-  </si>
-  <si>
-    <t>İş Hayatı ve İş Güvenliğine Hazırlık</t>
-  </si>
-  <si>
-    <t>İngilizce I</t>
+    <t>Gezgin Robotlara Giriş</t>
   </si>
   <si>
     <t>Mantıksal Tasarım ve Uygulamalar</t>
   </si>
   <si>
-    <t>Araştırma Problemleri</t>
-  </si>
-  <si>
-    <t>Staj II</t>
-  </si>
-  <si>
-    <t>Veri Yapıları ve Algoritmaları</t>
-  </si>
-  <si>
-    <t>Bitirme Çalışması</t>
-  </si>
-  <si>
-    <t>Atatürk İlkeleri ve İnkılap Tarihi I</t>
-  </si>
-  <si>
-    <t>Mikroişlemci Sistemleri</t>
-  </si>
-  <si>
-    <t>Matematik I</t>
-  </si>
-  <si>
-    <t>Bilgisayarlı Görmenin Temelleri</t>
-  </si>
-  <si>
-    <t>Ayrık Matematik</t>
-  </si>
-  <si>
-    <t>İşaret ve Sistemler</t>
-  </si>
-  <si>
-    <t>Staj I</t>
-  </si>
-  <si>
-    <t>Mobil Programlama</t>
-  </si>
-  <si>
-    <t>Robotlar için Matematik Temelleri</t>
-  </si>
-  <si>
-    <t>Bilgisayar Laboratuvarı I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Programlama I </t>
-  </si>
-  <si>
-    <t>Sayısal Yöntemler</t>
-  </si>
-  <si>
-    <t>Bilgisayar Ağları</t>
-  </si>
-  <si>
-    <t>Diferansiyel Denklemler</t>
-  </si>
-  <si>
-    <t>İşletim Sistemleri</t>
-  </si>
-  <si>
-    <t>Mühendisler için İstatistik</t>
-  </si>
-  <si>
-    <t>Türk Dili I</t>
-  </si>
-  <si>
-    <t>Fizik I</t>
-  </si>
-  <si>
-    <t>Biyoinformatiğe Giriş</t>
-  </si>
-  <si>
-    <t>Doğal Dil İşleme ve Metin Madenciliğine Giriş</t>
-  </si>
-  <si>
-    <t>Derin Öğrenmenin Temelleri</t>
-  </si>
-  <si>
-    <t>Veri Madenciliğine Giriş</t>
-  </si>
-  <si>
-    <t>Yazılım Proje Yönetimi</t>
-  </si>
-  <si>
-    <t>Gezgin Robotlara Giriş</t>
-  </si>
-  <si>
-    <t>Bilgisayar Semineri</t>
+    <t>Dr. Öğr. Üyesi Burak İnner</t>
+  </si>
+  <si>
+    <t>Doç. Dr. Meltem Kurt Pehlivanoğlu</t>
+  </si>
+  <si>
+    <t>Doç. Dr. Alev Mutlu</t>
+  </si>
+  <si>
+    <t>Doç. Dr. Pınar Onay Durdu</t>
+  </si>
+  <si>
+    <t>Dr. Öğr. Üyesi Furkan Göz</t>
+  </si>
+  <si>
+    <t>Ders Veren Bölüm Öğretim Elemanları</t>
+  </si>
+  <si>
+    <t>Prof. Dr. Sevinç İlhan Omurca</t>
+  </si>
+  <si>
+    <t>Doç. Dr. MİNE AYLİN BAYRAK</t>
+  </si>
+  <si>
+    <t>Prof. Dr. Selda Çalkavur</t>
+  </si>
+  <si>
+    <t>Dr. Öğr. Üyesi Fidan Kaya Gülağız</t>
+  </si>
+  <si>
+    <t>Öğr. Gör. Dr. Onur Gök</t>
+  </si>
+  <si>
+    <t>Arş. Gör. Dr. Gülcan Özkum</t>
+  </si>
+  <si>
+    <t>Prof. Dr. Suhap Şahin</t>
+  </si>
+  <si>
+    <t>Prof. Dr. Jale Süngü Yılmazkaya</t>
+  </si>
+  <si>
+    <t>Doç. Dr. Orhan Akbulut</t>
+  </si>
+  <si>
+    <t>Prof. Dr. Adnan Kavak</t>
+  </si>
+  <si>
+    <t>Öğr. Gör. Resul Özkan</t>
+  </si>
+  <si>
+    <t>Öğr. Gör. Ali SEZER</t>
   </si>
   <si>
     <t>Doç. Dr. Yücel Türker Ulutaş</t>
   </si>
   <si>
+    <t>Öğr. Gör. Şiva Koçak</t>
+  </si>
+  <si>
+    <t>Arş. Gör. Dr. Ayşe Gül Eker</t>
+  </si>
+  <si>
+    <t>Öğr. Gör. Uğur Yıldız</t>
+  </si>
+  <si>
     <t>Dr. Öğr. Üyesi Hikmetcan Özcan</t>
   </si>
   <si>
-    <t>Doç. Dr. Meltem Kurt Pehlivanoğlu</t>
-  </si>
-  <si>
     <t>Dr. Öğr. Üyesi Mehmet Ali Altuncu</t>
   </si>
   <si>
-    <t>Dr. Öğr. Üyesi Burak İnner</t>
-  </si>
-  <si>
-    <t>Dr. Öğr. Üyesi Furkan Göz</t>
-  </si>
-  <si>
-    <t>Öğr. Gör. Resul Özkan</t>
-  </si>
-  <si>
-    <t>Öğr. Gör. Ali SEZER</t>
-  </si>
-  <si>
-    <t>Dr. Öğr. Üyesi Fidan Kaya Gülağız</t>
-  </si>
-  <si>
-    <t>Ders Veren Bölüm Öğretim Elemanları</t>
-  </si>
-  <si>
-    <t>Prof. Dr. Suhap Şahin</t>
-  </si>
-  <si>
     <t>Öğr. Gör. Melih Yiğit</t>
   </si>
   <si>
-    <t>Prof. Dr. Selda Çalkavur</t>
-  </si>
-  <si>
-    <t>Doç. Dr. Orhan Akbulut</t>
-  </si>
-  <si>
-    <t>Doç. Dr. Alev Mutlu</t>
-  </si>
-  <si>
-    <t>Prof. Dr. Adnan Kavak</t>
-  </si>
-  <si>
-    <t>Öğr. Gör. Uğur Yıldız</t>
-  </si>
-  <si>
-    <t>Öğr. Gör. Dr. Onur Gök</t>
-  </si>
-  <si>
-    <t>Doç. Dr. MİNE AYLİN BAYRAK</t>
-  </si>
-  <si>
-    <t>Doç. Dr. Pınar Onay Durdu</t>
-  </si>
-  <si>
-    <t>Arş. Gör. Dr. Gülcan Özkum</t>
-  </si>
-  <si>
-    <t>Öğr. Gör. Şiva Koçak</t>
-  </si>
-  <si>
-    <t>Prof. Dr. Jale Süngü Yılmazkaya</t>
-  </si>
-  <si>
     <t>Dr. Öğr. Üyesi Burcu Kır Savaş</t>
   </si>
   <si>
-    <t>Prof. Dr. Sevinç İlhan Omurca</t>
-  </si>
-  <si>
-    <t>Arş. Gör. Dr. Ayşe Gül Eker</t>
-  </si>
-  <si>
-    <t>301, Büyük Amfi, EDA</t>
+    <t>a</t>
   </si>
   <si>
     <t>BİLGİSAYAR MÜHENDİSLİĞİ BÖLÜMÜ VİZE SINAV PROGRAMI</t>
@@ -696,7 +699,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -705,19 +708,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -725,76 +728,76 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -802,624 +805,606 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3"/>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3"/>
       <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3"/>
+      <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="3" t="s">
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="3"/>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3"/>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3"/>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3"/>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A18" s="3"/>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3"/>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="3"/>
+      <c r="A20" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E21" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3"/>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="A23" s="3"/>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3"/>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="3"/>
+      <c r="A25" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3"/>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3"/>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E27" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A28" s="3"/>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D28" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="E28" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3"/>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="E29" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3"/>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E30" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="3"/>
+      <c r="A31" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="E31" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3"/>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D32" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="3"/>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" t="s">
         <v>65</v>
       </c>
-      <c r="E32" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" t="s">
-        <v>43</v>
-      </c>
-      <c r="D33" t="s">
-        <v>73</v>
-      </c>
       <c r="E33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3"/>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D34" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E34" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3"/>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D35" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E35" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3"/>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3"/>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
         <v>7</v>
       </c>
-      <c r="B38" t="s">
-        <v>8</v>
-      </c>
       <c r="C38" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D38" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="E38" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3"/>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D39" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E39" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3"/>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D40" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E40" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3"/>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D41" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E41" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="8">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A25:A30"/>
+    <mergeCell ref="A31:A37"/>
     <mergeCell ref="A38:A41"/>
   </mergeCells>
-  <conditionalFormatting sqref="A13:A17">
+  <conditionalFormatting sqref="A14:A19">
     <cfRule type="notContainsBlanks" dxfId="1" priority="8">
-      <formula>LEN(TRIM(A13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13:B17">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:B19">
     <cfRule type="notContainsBlanks" dxfId="1" priority="9">
-      <formula>LEN(TRIM(A13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13:E17">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:E19">
     <cfRule type="notContainsBlanks" dxfId="0" priority="7">
-      <formula>LEN(TRIM(A13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18:A22">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:A24">
     <cfRule type="notContainsBlanks" dxfId="1" priority="11">
-      <formula>LEN(TRIM(A18))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18:B22">
+      <formula>LEN(TRIM(A20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:B24">
     <cfRule type="notContainsBlanks" dxfId="1" priority="12">
-      <formula>LEN(TRIM(A18))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18:E22">
+      <formula>LEN(TRIM(A20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:E24">
     <cfRule type="notContainsBlanks" dxfId="0" priority="10">
-      <formula>LEN(TRIM(A18))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23:A27">
+      <formula>LEN(TRIM(A20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25:A30">
     <cfRule type="notContainsBlanks" dxfId="1" priority="14">
-      <formula>LEN(TRIM(A23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23:B27">
+      <formula>LEN(TRIM(A25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25:B30">
     <cfRule type="notContainsBlanks" dxfId="1" priority="15">
-      <formula>LEN(TRIM(A23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23:E27">
+      <formula>LEN(TRIM(A25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25:E30">
     <cfRule type="notContainsBlanks" dxfId="0" priority="13">
-      <formula>LEN(TRIM(A23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28:A32">
+      <formula>LEN(TRIM(A25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31:A37">
     <cfRule type="notContainsBlanks" dxfId="1" priority="17">
-      <formula>LEN(TRIM(A28))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28:B32">
+      <formula>LEN(TRIM(A31))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31:B37">
     <cfRule type="notContainsBlanks" dxfId="1" priority="18">
-      <formula>LEN(TRIM(A28))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28:E32">
+      <formula>LEN(TRIM(A31))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31:E37">
     <cfRule type="notContainsBlanks" dxfId="0" priority="16">
-      <formula>LEN(TRIM(A28))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33:A37">
+      <formula>LEN(TRIM(A31))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:A41">
     <cfRule type="notContainsBlanks" dxfId="1" priority="20">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33:B37">
+      <formula>LEN(TRIM(A38))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:B41">
     <cfRule type="notContainsBlanks" dxfId="1" priority="21">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33:E37">
+      <formula>LEN(TRIM(A38))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:E41">
     <cfRule type="notContainsBlanks" dxfId="0" priority="19">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38:A41">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="23">
-      <formula>LEN(TRIM(A38))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38:B41">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="24">
-      <formula>LEN(TRIM(A38))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38:E41">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="22">
       <formula>LEN(TRIM(A38))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1438,17 +1423,17 @@
       <formula>LEN(TRIM(A3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8:A12">
+  <conditionalFormatting sqref="A8:A13">
     <cfRule type="notContainsBlanks" dxfId="1" priority="5">
       <formula>LEN(TRIM(A8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8:B12">
+  <conditionalFormatting sqref="A8:B13">
     <cfRule type="notContainsBlanks" dxfId="1" priority="6">
       <formula>LEN(TRIM(A8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8:E12">
+  <conditionalFormatting sqref="A8:E13">
     <cfRule type="notContainsBlanks" dxfId="0" priority="4">
       <formula>LEN(TRIM(A8))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekends exclude part entegrated to created program func.
</commit_message>
<xml_diff>
--- a/sinav_programi.xlsx
+++ b/sinav_programi.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="78">
   <si>
     <t>2025-09-29</t>
   </si>
@@ -31,10 +31,19 @@
     <t>2025-10-03</t>
   </si>
   <si>
-    <t>2025-10-04</t>
-  </si>
-  <si>
-    <t>2025-10-05</t>
+    <t>2025-10-06</t>
+  </si>
+  <si>
+    <t>2025-10-07</t>
+  </si>
+  <si>
+    <t>2025-10-08</t>
+  </si>
+  <si>
+    <t>2025-10-09</t>
+  </si>
+  <si>
+    <t>2025-10-10</t>
   </si>
   <si>
     <t>09:00</t>
@@ -49,208 +58,175 @@
     <t>13:30</t>
   </si>
   <si>
-    <t>15:00</t>
-  </si>
-  <si>
-    <t>16:30</t>
-  </si>
-  <si>
-    <t>18:00</t>
+    <t>Lineer Cebir</t>
+  </si>
+  <si>
+    <t>Matematik I</t>
+  </si>
+  <si>
+    <t>Derin Öğrenmenin Temelleri</t>
+  </si>
+  <si>
+    <t>İşaret ve Sistemler</t>
+  </si>
+  <si>
+    <t>İşletim Sistemleri</t>
+  </si>
+  <si>
+    <t>İngilizce I</t>
+  </si>
+  <si>
+    <t>Doğal Dil İşleme ve Metin Madenciliğine Giriş</t>
+  </si>
+  <si>
+    <t>Nesneye Yönelik Programlama</t>
+  </si>
+  <si>
+    <t>Mikroişlemci Sistemleri</t>
+  </si>
+  <si>
+    <t>Mobil Programlama</t>
+  </si>
+  <si>
+    <t>Araştırma Problemleri</t>
+  </si>
+  <si>
+    <t>Biyoinformatiğe Giriş</t>
+  </si>
+  <si>
+    <t>Bilgisayar Mühendisliğine Giriş</t>
+  </si>
+  <si>
+    <t>Bilgi Güvenliği ve Kriptografi</t>
+  </si>
+  <si>
+    <t>Bilgisayar Semineri</t>
+  </si>
+  <si>
+    <t>Mantıksal Tasarım ve Uygulamalar</t>
+  </si>
+  <si>
+    <t>Bilgisayar Ağları</t>
+  </si>
+  <si>
+    <t>Sayısal Yöntemler</t>
+  </si>
+  <si>
+    <t>Yazılım Proje Yönetimi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programlama I </t>
+  </si>
+  <si>
+    <t>Türk Dili I</t>
   </si>
   <si>
     <t>Robotlar için Matematik Temelleri</t>
   </si>
   <si>
-    <t>Mikroişlemci Sistemleri</t>
+    <t>Fizik I</t>
+  </si>
+  <si>
+    <t>Diferansiyel Denklemler</t>
+  </si>
+  <si>
+    <t>Veri Yapıları ve Algoritmaları</t>
+  </si>
+  <si>
+    <t>Programlanabilir Yapılar</t>
+  </si>
+  <si>
+    <t>Veri Madenciliğine Giriş</t>
+  </si>
+  <si>
+    <t>Atatürk İlkeleri ve İnkılap Tarihi I</t>
+  </si>
+  <si>
+    <t>Gezgin Robotlara Giriş</t>
   </si>
   <si>
     <t>Ayrık Matematik</t>
   </si>
   <si>
-    <t>Bilgisayar Ağları</t>
-  </si>
-  <si>
-    <t>Doğal Dil İşleme ve Metin Madenciliğine Giriş</t>
-  </si>
-  <si>
-    <t>Araştırma Problemleri</t>
-  </si>
-  <si>
-    <t>Veri Madenciliğine Giriş</t>
-  </si>
-  <si>
-    <t>Sayısal Yöntemler</t>
-  </si>
-  <si>
-    <t>Matematik I</t>
-  </si>
-  <si>
-    <t>Staj II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Programlama I </t>
-  </si>
-  <si>
-    <t>Diferansiyel Denklemler</t>
-  </si>
-  <si>
-    <t>Veri Yapıları ve Algoritmaları</t>
-  </si>
-  <si>
-    <t>Fizik I</t>
-  </si>
-  <si>
-    <t>Mühendisler için İstatistik</t>
-  </si>
-  <si>
-    <t>İşaret ve Sistemler</t>
-  </si>
-  <si>
-    <t>İş Hayatı ve İş Güvenliğine Hazırlık</t>
-  </si>
-  <si>
-    <t>İngilizce I</t>
-  </si>
-  <si>
-    <t>Lineer Cebir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Programlama Laboratuvarı - I </t>
-  </si>
-  <si>
     <t>Bitirme Çalışması</t>
   </si>
   <si>
-    <t>Yazılım Proje Yönetimi</t>
-  </si>
-  <si>
-    <t>Türk Dili I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yazılım Laboratuvarı I </t>
-  </si>
-  <si>
-    <t>Bilgisayar Laboratuvarı I</t>
-  </si>
-  <si>
-    <t>Bilgi Güvenliği ve Kriptografi</t>
-  </si>
-  <si>
-    <t>Biyoinformatiğe Giriş</t>
-  </si>
-  <si>
-    <t>Bilgisayar Semineri</t>
-  </si>
-  <si>
-    <t>Mobil Programlama</t>
-  </si>
-  <si>
-    <t>Nesneye Yönelik Programlama</t>
-  </si>
-  <si>
-    <t>İşletim Sistemleri</t>
-  </si>
-  <si>
     <t>Bilgisayarlı Görmenin Temelleri</t>
   </si>
   <si>
-    <t>Bilgisayar Mühendisliğine Giriş</t>
-  </si>
-  <si>
-    <t>Atatürk İlkeleri ve İnkılap Tarihi I</t>
-  </si>
-  <si>
-    <t>Derin Öğrenmenin Temelleri</t>
-  </si>
-  <si>
-    <t>Staj I</t>
-  </si>
-  <si>
-    <t>Programlanabilir Yapılar</t>
-  </si>
-  <si>
-    <t>Gezgin Robotlara Giriş</t>
-  </si>
-  <si>
-    <t>Mantıksal Tasarım ve Uygulamalar</t>
+    <t>Doç. Dr. Yücel Türker Ulutaş</t>
+  </si>
+  <si>
+    <t>Prof. Dr. Selda Çalkavur</t>
+  </si>
+  <si>
+    <t>Dr. Öğr. Üyesi Burcu Kır Savaş</t>
+  </si>
+  <si>
+    <t>Prof. Dr. Adnan Kavak</t>
+  </si>
+  <si>
+    <t>Prof. Dr. Suhap Şahin</t>
+  </si>
+  <si>
+    <t>Öğr. Gör. Ali SEZER</t>
+  </si>
+  <si>
+    <t>Dr. Öğr. Üyesi Furkan Göz</t>
+  </si>
+  <si>
+    <t>Dr. Öğr. Üyesi Hikmetcan Özcan</t>
+  </si>
+  <si>
+    <t>Doç. Dr. Meltem Kurt Pehlivanoğlu</t>
+  </si>
+  <si>
+    <t>Öğr. Gör. Uğur Yıldız</t>
+  </si>
+  <si>
+    <t>Ders Veren Bölüm Öğretim Elemanları</t>
+  </si>
+  <si>
+    <t>Doç. Dr. Alev Mutlu</t>
+  </si>
+  <si>
+    <t>Dr. Öğr. Üyesi Mehmet Ali Altuncu</t>
+  </si>
+  <si>
+    <t>Arş. Gör. Dr. Ayşe Gül Eker</t>
+  </si>
+  <si>
+    <t>Dr. Öğr. Üyesi Fidan Kaya Gülağız</t>
+  </si>
+  <si>
+    <t>Doç. Dr. Pınar Onay Durdu</t>
+  </si>
+  <si>
+    <t>Doç. Dr. MİNE AYLİN BAYRAK</t>
+  </si>
+  <si>
+    <t>Öğr. Gör. Dr. Onur Gök</t>
+  </si>
+  <si>
+    <t>Öğr. Gör. Şiva Koçak</t>
   </si>
   <si>
     <t>Dr. Öğr. Üyesi Burak İnner</t>
   </si>
   <si>
-    <t>Doç. Dr. Meltem Kurt Pehlivanoğlu</t>
-  </si>
-  <si>
-    <t>Doç. Dr. Alev Mutlu</t>
-  </si>
-  <si>
-    <t>Doç. Dr. Pınar Onay Durdu</t>
-  </si>
-  <si>
-    <t>Dr. Öğr. Üyesi Furkan Göz</t>
-  </si>
-  <si>
-    <t>Ders Veren Bölüm Öğretim Elemanları</t>
+    <t>Prof. Dr. Jale Süngü Yılmazkaya</t>
+  </si>
+  <si>
+    <t>Arş. Gör. Dr. Gülcan Özkum</t>
   </si>
   <si>
     <t>Prof. Dr. Sevinç İlhan Omurca</t>
   </si>
   <si>
-    <t>Doç. Dr. MİNE AYLİN BAYRAK</t>
-  </si>
-  <si>
-    <t>Prof. Dr. Selda Çalkavur</t>
-  </si>
-  <si>
-    <t>Dr. Öğr. Üyesi Fidan Kaya Gülağız</t>
-  </si>
-  <si>
-    <t>Öğr. Gör. Dr. Onur Gök</t>
-  </si>
-  <si>
-    <t>Arş. Gör. Dr. Gülcan Özkum</t>
-  </si>
-  <si>
-    <t>Prof. Dr. Suhap Şahin</t>
-  </si>
-  <si>
-    <t>Prof. Dr. Jale Süngü Yılmazkaya</t>
+    <t>Öğr. Gör. Melih Yiğit</t>
   </si>
   <si>
     <t>Doç. Dr. Orhan Akbulut</t>
-  </si>
-  <si>
-    <t>Prof. Dr. Adnan Kavak</t>
-  </si>
-  <si>
-    <t>Öğr. Gör. Resul Özkan</t>
-  </si>
-  <si>
-    <t>Öğr. Gör. Ali SEZER</t>
-  </si>
-  <si>
-    <t>Doç. Dr. Yücel Türker Ulutaş</t>
-  </si>
-  <si>
-    <t>Öğr. Gör. Şiva Koçak</t>
-  </si>
-  <si>
-    <t>Arş. Gör. Dr. Ayşe Gül Eker</t>
-  </si>
-  <si>
-    <t>Öğr. Gör. Uğur Yıldız</t>
-  </si>
-  <si>
-    <t>Dr. Öğr. Üyesi Hikmetcan Özcan</t>
-  </si>
-  <si>
-    <t>Dr. Öğr. Üyesi Mehmet Ali Altuncu</t>
-  </si>
-  <si>
-    <t>Öğr. Gör. Melih Yiğit</t>
-  </si>
-  <si>
-    <t>Dr. Öğr. Üyesi Burcu Kır Savaş</t>
   </si>
   <si>
     <t>a</t>
@@ -686,7 +662,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -699,7 +675,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -708,19 +684,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -728,50 +704,52 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -779,10 +757,10 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -794,153 +772,155 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="A8" s="3"/>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3"/>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3"/>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3"/>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3"/>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3"/>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="3"/>
+      <c r="A17" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -948,10 +928,10 @@
         <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -963,10 +943,10 @@
         <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -978,61 +958,63 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
         <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E20" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
         <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3"/>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
         <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="E22" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="3"/>
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="B23" t="s">
         <v>10</v>
       </c>
@@ -1040,10 +1022,10 @@
         <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E23" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1055,387 +1037,330 @@
         <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E24" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="A25" s="3"/>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C25" t="s">
         <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="3"/>
+      <c r="A26" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C26" t="s">
         <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3"/>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C27" t="s">
         <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3"/>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
         <v>39</v>
       </c>
       <c r="D28" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="3"/>
+      <c r="A29" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
         <v>40</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3"/>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
         <v>41</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E30" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A31" s="3"/>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C31" t="s">
         <v>42</v>
       </c>
       <c r="D31" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E31" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="3"/>
+      <c r="A32" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C32" t="s">
         <v>43</v>
       </c>
       <c r="D32" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="E32" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3"/>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C33" t="s">
         <v>44</v>
       </c>
       <c r="D33" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E33" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3"/>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C34" t="s">
         <v>45</v>
       </c>
       <c r="D34" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="3"/>
-      <c r="B35" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" t="s">
-        <v>46</v>
-      </c>
-      <c r="D35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E35" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="3"/>
-      <c r="B36" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" t="s">
-        <v>47</v>
-      </c>
-      <c r="D36" t="s">
-        <v>77</v>
-      </c>
-      <c r="E36" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="3"/>
-      <c r="B37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" t="s">
-        <v>48</v>
-      </c>
-      <c r="D37" t="s">
-        <v>78</v>
-      </c>
-      <c r="E37" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
-        <v>49</v>
-      </c>
-      <c r="D38" t="s">
-        <v>62</v>
-      </c>
-      <c r="E38" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="3"/>
-      <c r="B39" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" t="s">
-        <v>50</v>
-      </c>
-      <c r="D39" t="s">
-        <v>76</v>
-      </c>
-      <c r="E39" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="3"/>
-      <c r="B40" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" t="s">
-        <v>51</v>
-      </c>
-      <c r="D40" t="s">
-        <v>53</v>
-      </c>
-      <c r="E40" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="3"/>
-      <c r="B41" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D41" t="s">
-        <v>62</v>
-      </c>
-      <c r="E41" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="11">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A25:A30"/>
-    <mergeCell ref="A31:A37"/>
-    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A32:A34"/>
   </mergeCells>
-  <conditionalFormatting sqref="A14:A19">
+  <conditionalFormatting sqref="A10:A13">
     <cfRule type="notContainsBlanks" dxfId="1" priority="8">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:B13">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="9">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:E13">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="7">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:A16">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="11">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14:B19">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="9">
+  <conditionalFormatting sqref="A14:B16">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="12">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14:E19">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="7">
+  <conditionalFormatting sqref="A14:E16">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="10">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:A24">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="11">
+  <conditionalFormatting sqref="A17:A19">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="14">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17:B19">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="15">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17:E19">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="13">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:A22">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="17">
       <formula>LEN(TRIM(A20))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:B24">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="12">
+  <conditionalFormatting sqref="A20:B22">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="18">
       <formula>LEN(TRIM(A20))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:E24">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="10">
+  <conditionalFormatting sqref="A20:E22">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="16">
       <formula>LEN(TRIM(A20))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A25:A30">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="14">
-      <formula>LEN(TRIM(A25))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25:B30">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="15">
-      <formula>LEN(TRIM(A25))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25:E30">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="13">
-      <formula>LEN(TRIM(A25))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31:A37">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="17">
-      <formula>LEN(TRIM(A31))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31:B37">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="18">
-      <formula>LEN(TRIM(A31))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31:E37">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="16">
-      <formula>LEN(TRIM(A31))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38:A41">
+  <conditionalFormatting sqref="A23:A25">
     <cfRule type="notContainsBlanks" dxfId="1" priority="20">
-      <formula>LEN(TRIM(A38))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38:B41">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23:B25">
     <cfRule type="notContainsBlanks" dxfId="1" priority="21">
-      <formula>LEN(TRIM(A38))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38:E41">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23:E25">
     <cfRule type="notContainsBlanks" dxfId="0" priority="19">
-      <formula>LEN(TRIM(A38))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A7">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:A28">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="23">
+      <formula>LEN(TRIM(A26))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:B28">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="24">
+      <formula>LEN(TRIM(A26))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:E28">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="22">
+      <formula>LEN(TRIM(A26))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:A31">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="26">
+      <formula>LEN(TRIM(A29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:B31">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="27">
+      <formula>LEN(TRIM(A29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:E31">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="25">
+      <formula>LEN(TRIM(A29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32:A34">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="29">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32:B34">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="30">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32:E34">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="28">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:A5">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:B7">
+  <conditionalFormatting sqref="A3:B5">
     <cfRule type="notContainsBlanks" dxfId="1" priority="3">
       <formula>LEN(TRIM(A3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:E7">
+  <conditionalFormatting sqref="A3:E5">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8:A13">
+  <conditionalFormatting sqref="A6:A9">
     <cfRule type="notContainsBlanks" dxfId="1" priority="5">
-      <formula>LEN(TRIM(A8))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8:B13">
+      <formula>LEN(TRIM(A6))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:B9">
     <cfRule type="notContainsBlanks" dxfId="1" priority="6">
-      <formula>LEN(TRIM(A8))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8:E13">
+      <formula>LEN(TRIM(A6))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:E9">
     <cfRule type="notContainsBlanks" dxfId="0" priority="4">
-      <formula>LEN(TRIM(A8))&gt;0</formula>
+      <formula>LEN(TRIM(A6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>